<commit_message>
update details of Excel - 230306
</commit_message>
<xml_diff>
--- a/2023_Q1/2023-Q1_羽球季打費用明細.xlsx
+++ b/2023_Q1/2023-Q1_羽球季打費用明細.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alias\Documents\Private\2023_Q1_週一豐東羽球團\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alias\Documents\Docs\Private\週一豐東羽球團\2023_Q1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849402CD-A412-4836-A4DA-4AE095BEE5C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E332A57E-3253-407F-8AF8-D2EAC0BEAC0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{8981F119-1F50-4E2E-B5FC-EDE94F1AD592}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{8981F119-1F50-4E2E-B5FC-EDE94F1AD592}"/>
   </bookViews>
   <sheets>
     <sheet name="2023Q1羽球季費資訊" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="64">
   <si>
     <t>[4次] 12/05,12,19,26</t>
   </si>
@@ -258,10 +258,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>冠村 臨打費 (未入帳)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>現金 偉群友(嘉穎) @鉉竣  @林丞斌 (夜市代收)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -271,6 +267,18 @@
   </si>
   <si>
     <t>=SUM(B2:C36)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>現金 冠村 臨打費 (夜市代收)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>現金 Chia Ying  臨打費</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>現金 香菇*2 臨打費</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -810,9 +818,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D35F76AE-921C-47CE-BB7E-B46F0098B109}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
-    </sheetView>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -995,10 +1001,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C507093-BF74-439E-A89C-015FFCC1218B}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1297,7 +1303,7 @@
         <v>510</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1320,7 +1326,7 @@
         <v>340</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1363,23 +1369,45 @@
       </c>
       <c r="B31" s="16"/>
       <c r="C31" s="17">
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C32" s="10"/>
+      <c r="A32" s="6">
+        <v>44991</v>
+      </c>
+      <c r="C32" s="10">
+        <v>170</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="15"/>
+      <c r="A33" s="15">
+        <v>44991</v>
+      </c>
       <c r="B33" s="16"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="18"/>
+      <c r="C33" s="17">
+        <v>170</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C34" s="10"/>
+      <c r="A34" s="6">
+        <v>44991</v>
+      </c>
+      <c r="C34" s="10">
+        <v>340</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="15"/>
@@ -1387,20 +1415,44 @@
       <c r="C35" s="17"/>
       <c r="D35" s="18"/>
     </row>
-    <row r="36" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C36" s="10"/>
     </row>
-    <row r="37" spans="1:4" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="15"/>
+      <c r="B37" s="16"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="18"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C38" s="10"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="15"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="18"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C40" s="10"/>
+    </row>
+    <row r="41" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="15"/>
+      <c r="B41" s="16"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="18"/>
+    </row>
+    <row r="42" spans="1:4" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B37" s="9"/>
-      <c r="C37" s="9">
-        <f>SUM(B2:C36)</f>
-        <v>3280</v>
-      </c>
-      <c r="D37" s="23" t="s">
-        <v>61</v>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9">
+        <f>SUM(B2:C41)</f>
+        <v>4130</v>
+      </c>
+      <c r="D42" s="23" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update deatils of 2023Q2 and close 2023Q1 - 230313
</commit_message>
<xml_diff>
--- a/2023_Q1/2023-Q1_羽球季打費用明細.xlsx
+++ b/2023_Q1/2023-Q1_羽球季打費用明細.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alias\Documents\Docs\Private\週一豐東羽球團\2023_Q1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E332A57E-3253-407F-8AF8-D2EAC0BEAC0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDA3BC8-0AB0-42CD-8A2D-98039C2F4B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{8981F119-1F50-4E2E-B5FC-EDE94F1AD592}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{8981F119-1F50-4E2E-B5FC-EDE94F1AD592}"/>
   </bookViews>
   <sheets>
     <sheet name="2023Q1羽球季費資訊" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="68">
   <si>
     <t>[4次] 12/05,12,19,26</t>
   </si>
@@ -202,10 +202,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>現金 @Ivy GOSEN GFN60 新球一筒</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">=$142*10次 </t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -266,10 +262,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>=SUM(B2:C36)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>現金 冠村 臨打費 (夜市代收)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -279,6 +271,29 @@
   </si>
   <si>
     <t>現金 香菇*2 臨打費</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>現金 @Ivy VOLAR 10 新球 $330 六筒</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>現金 @Ivy GOSEN GFN60 新球 $420 一筒</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>現金 @Chia Ying 臨打費</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>現金 @鉉竣 臨打費</t>
+  </si>
+  <si>
+    <t>現金 @小幫手香菇+2 臨打費</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>==SUM(B2:C41)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -930,7 +945,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B20" s="11">
         <f>B18/12</f>
@@ -974,7 +989,7 @@
         <v>1420</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1004,7 +1019,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1017,7 +1032,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B1" s="20" t="s">
         <v>13</v>
@@ -1142,7 +1157,7 @@
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="18" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1188,7 +1203,7 @@
         <v>1420</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1199,7 +1214,7 @@
         <v>170</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1211,7 +1226,7 @@
         <v>100</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1222,7 +1237,7 @@
         <v>300</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1234,7 +1249,7 @@
         <v>40</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1245,7 +1260,7 @@
         <v>170</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1257,7 +1272,7 @@
         <v>170</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1268,7 +1283,7 @@
         <v>170</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1280,7 +1295,7 @@
         <v>170</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1291,7 +1306,7 @@
         <v>170</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1303,7 +1318,7 @@
         <v>510</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1314,7 +1329,7 @@
         <v>170</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1326,7 +1341,7 @@
         <v>340</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1337,7 +1352,7 @@
         <v>170</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1349,7 +1364,7 @@
         <v>170</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1372,7 +1387,7 @@
         <v>170</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1383,7 +1398,7 @@
         <v>170</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1395,7 +1410,7 @@
         <v>170</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1406,35 +1421,77 @@
         <v>340</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="15"/>
-      <c r="B35" s="16"/>
+      <c r="A35" s="15">
+        <v>44998</v>
+      </c>
+      <c r="B35" s="16">
+        <v>-1980</v>
+      </c>
       <c r="C35" s="17"/>
-      <c r="D35" s="18"/>
+      <c r="D35" s="18" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C36" s="10"/>
+      <c r="A36" s="6">
+        <v>44998</v>
+      </c>
+      <c r="C36" s="10">
+        <v>150</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="15"/>
+      <c r="A37" s="15">
+        <v>44998</v>
+      </c>
       <c r="B37" s="16"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="18"/>
+      <c r="C37" s="17">
+        <v>150</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C38" s="10"/>
+      <c r="A38" s="6">
+        <v>44998</v>
+      </c>
+      <c r="C38" s="10">
+        <v>150</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="15"/>
+      <c r="A39" s="15">
+        <v>44998</v>
+      </c>
       <c r="B39" s="16"/>
-      <c r="C39" s="17"/>
-      <c r="D39" s="18"/>
+      <c r="C39" s="17">
+        <v>150</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C40" s="10"/>
+      <c r="A40" s="6">
+        <v>44998</v>
+      </c>
+      <c r="C40" s="10">
+        <v>300</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="41" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="15"/>
@@ -1449,10 +1506,10 @@
       <c r="B42" s="9"/>
       <c r="C42" s="9">
         <f>SUM(B2:C41)</f>
-        <v>4130</v>
+        <v>3050</v>
       </c>
       <c r="D42" s="23" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>